<commit_message>
MOD:Changes in process description
</commit_message>
<xml_diff>
--- a/cl.bancochile.fdd.master.cmf/src/resources/pd/PD_tbl_cmf_Activos1_mes.xlsx
+++ b/cl.bancochile.fdd.master.cmf/src/resources/pd/PD_tbl_cmf_Activos1_mes.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1220212.SOAM\Desktop\PreSales\Banco de Chile\2020-11-28 - Gobierno de Datos - Monovendor Células Ágiles Datalake\FDs and PDs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0E1B11-B584-4B6D-9516-E5F9AC9E0555}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6C6015-8B87-4365-B4E4-6A37B32EBF80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Format Details" sheetId="1" r:id="rId1"/>
+    <sheet name="DataQuality - Validaciones" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
   <si>
     <t>Institucion</t>
   </si>
@@ -160,6 +161,27 @@
   </si>
   <si>
     <t>monotonically_increasing_id()</t>
+  </si>
+  <si>
+    <t>Validations</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>Activos Bancos 1 cross Activos Bancos 2</t>
+  </si>
+  <si>
+    <t>activos1 . Column B = activos 2 . Column Z</t>
+  </si>
+  <si>
+    <t>Activos Bancos 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column K  
+      minimum value 0 
+      maximum value 100.000.000
+</t>
   </si>
 </sst>
 </file>
@@ -197,7 +219,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -216,6 +238,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -299,7 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -316,17 +350,36 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -611,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:D27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -624,10 +677,10 @@
   <sheetData>
     <row r="1" spans="2:4" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="4" t="s">
@@ -660,16 +713,16 @@
     <row r="7" spans="2:4" ht="15.75" customHeight="1">
       <c r="B7" s="6"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" spans="2:4" ht="15.75" customHeight="1">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="14" t="s">
         <v>44</v>
       </c>
     </row>
@@ -685,7 +738,7 @@
       <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="8" t="s">
         <v>42</v>
       </c>
     </row>
@@ -696,7 +749,7 @@
       <c r="C11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -707,7 +760,7 @@
       <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -718,7 +771,7 @@
       <c r="C13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -729,7 +782,7 @@
       <c r="C14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -740,7 +793,7 @@
       <c r="C15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -751,7 +804,7 @@
       <c r="C16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -762,7 +815,7 @@
       <c r="C17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -773,7 +826,7 @@
       <c r="C18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -784,7 +837,7 @@
       <c r="C19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -795,7 +848,7 @@
       <c r="C20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -806,7 +859,7 @@
       <c r="C21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -817,7 +870,7 @@
       <c r="C22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -828,7 +881,7 @@
       <c r="C23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -839,7 +892,7 @@
       <c r="C24" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -850,7 +903,7 @@
       <c r="C25" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -863,4 +916,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88D84555-B439-49C6-832D-3FD5CF5335F5}">
+  <dimension ref="B2:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="85.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3">
+      <c r="B2" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="60">
+      <c r="B4" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>